<commit_message>
added waste resources and finished utility files
</commit_message>
<xml_diff>
--- a/data/resource_data.xlsx
+++ b/data/resource_data.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>R23</t>
   </si>
@@ -178,6 +178,36 @@
   </si>
   <si>
     <t>R26X</t>
+  </si>
+  <si>
+    <t>R2X</t>
+  </si>
+  <si>
+    <t>R3X</t>
+  </si>
+  <si>
+    <t>R4X</t>
+  </si>
+  <si>
+    <t>R5X</t>
+  </si>
+  <si>
+    <t>R6X</t>
+  </si>
+  <si>
+    <t>timber wastre</t>
+  </si>
+  <si>
+    <t>metallic elements waste</t>
+  </si>
+  <si>
+    <t>land waste</t>
+  </si>
+  <si>
+    <t>REC waste</t>
+  </si>
+  <si>
+    <t>FEC waste</t>
   </si>
 </sst>
 </file>
@@ -540,7 +570,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -823,6 +853,61 @@
         <v>41</v>
       </c>
     </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="3">
+        <v>-0.4</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3">
+        <v>-0.2</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="3">
+        <v>-0.3</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="3">
+        <v>-0.1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
rewriting the state quality functions
</commit_message>
<xml_diff>
--- a/data/resource_data.xlsx
+++ b/data/resource_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludwik/AI-Spring-2021/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellywolfe/PycharmProjects/AI-Spring-2021/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C7120E-667B-714A-B0D7-8D5D93D20842}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79719A3B-9F50-3448-8C33-1CBEDA3C3D8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12480" yWindow="460" windowWidth="16320" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>R23</t>
   </si>
@@ -202,6 +202,12 @@
   </si>
   <si>
     <t>Names</t>
+  </si>
+  <si>
+    <t>R7X</t>
+  </si>
+  <si>
+    <t>Water Waste</t>
   </si>
 </sst>
 </file>
@@ -559,15 +565,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -597,7 +603,7 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
@@ -605,291 +611,305 @@
     </row>
     <row r="4" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>-0.1</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>-0.1</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B10">
-        <v>0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>-0.1</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>59</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B15">
-        <v>0.8</v>
+        <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16">
-        <v>0.7</v>
+        <v>-0.2</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B17">
-        <v>-0.2</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>-0.1</v>
+        <v>-0.2</v>
       </c>
       <c r="C18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="B19">
-        <v>-0.3</v>
+        <v>5</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="B21">
-        <v>-0.4</v>
+        <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22">
-        <v>-0.5</v>
+        <v>-0.1</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="B23">
-        <v>-0.5</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24">
-        <v>-0.2</v>
+        <v>-0.1</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="B25">
-        <v>-0.4</v>
+        <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B26">
-        <v>-0.2</v>
+        <v>-0.3</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B27">
-        <v>-0.2</v>
+        <v>10</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B28">
-        <v>-0.3</v>
+        <v>-0.2</v>
       </c>
       <c r="C28" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B29">
-        <v>-0.1</v>
+        <v>10</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>-0.2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C30">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
added the extra transformations to world.py and resource_data.xlsx
</commit_message>
<xml_diff>
--- a/data/resource_data.xlsx
+++ b/data/resource_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kellywolfe/PycharmProjects/AI-Spring-2021/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/regansiems/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E45265C-E59C-AF40-9109-FFE3D8ED3C18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073E8B23-8699-3541-A5BC-673433EB6742}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="500" windowWidth="16320" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13560" yWindow="500" windowWidth="14260" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>R23</t>
   </si>
@@ -105,25 +105,85 @@
     <t>R25</t>
   </si>
   <si>
-    <t>Fertilizer</t>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>R5</t>
   </si>
   <si>
     <t>R25X</t>
   </si>
   <si>
-    <t>FertilizerWaste</t>
+    <t>RenewableEnergy</t>
   </si>
   <si>
     <t>R26</t>
   </si>
   <si>
-    <t>Farm</t>
-  </si>
-  <si>
     <t>R26X</t>
   </si>
   <si>
-    <t>FarmWaste</t>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>WeaponsWaste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Military </t>
+  </si>
+  <si>
+    <t>MilitaryWaste</t>
+  </si>
+  <si>
+    <t>Medicine</t>
+  </si>
+  <si>
+    <t>MedicineWaste</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>R27X</t>
+  </si>
+  <si>
+    <t>R28</t>
+  </si>
+  <si>
+    <t>R28X</t>
+  </si>
+  <si>
+    <t>Telecommunications</t>
+  </si>
+  <si>
+    <t>TelecommunicationsWaste</t>
+  </si>
+  <si>
+    <t>Transportation</t>
+  </si>
+  <si>
+    <t>TransportationWaste</t>
+  </si>
+  <si>
+    <t>R29</t>
+  </si>
+  <si>
+    <t>R29X</t>
+  </si>
+  <si>
+    <t>R30</t>
+  </si>
+  <si>
+    <t>R30X</t>
+  </si>
+  <si>
+    <t>FossilEnergyWaste</t>
+  </si>
+  <si>
+    <t>FossilEnergy</t>
   </si>
 </sst>
 </file>
@@ -481,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -538,138 +598,248 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="B6">
-        <v>-0.1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7">
         <v>1</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>-0.25</v>
+        <v>-0.1</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>-0.25</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>-0.25</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>-0.25</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
+      <c r="C14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16">
+        <v>-0.5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>31</v>
       </c>
-      <c r="B16">
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>-0.4</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19">
+        <v>3</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>-0.5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21">
+        <v>5</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22">
         <v>-0.25</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>32</v>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23">
+        <v>2.5</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24">
+        <v>-0.15</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25">
+        <v>2.5</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>-0.45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C12">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C14">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>